<commit_message>
Pre-trial 62 bugs ready for 8/16/2021.
</commit_message>
<xml_diff>
--- a/avbernat_working_on/Dispersal/Summer_2021/windaq_processing/data/masterlist.xlsx
+++ b/avbernat_working_on/Dispersal/Summer_2021/windaq_processing/data/masterlist.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/anastasiabernat/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/anastasiabernat/Desktop/git_repositories/SBB-dispersal/avbernat_working_on/Dispersal/Summer_2021/windaq_processing/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1CC2959-20E4-BF42-8DA3-817594AF4CB6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EBD1001-BEEF-1643-9368-47191AABD480}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="760" yWindow="500" windowWidth="28040" windowHeight="16680" xr2:uid="{836CA092-02C0-B74E-BDA7-EEABC1742BC7}"/>
+    <workbookView xWindow="760" yWindow="500" windowWidth="28040" windowHeight="16640" xr2:uid="{836CA092-02C0-B74E-BDA7-EEABC1742BC7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2008" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2028" uniqueCount="34">
   <si>
     <t>ID</t>
   </si>
@@ -122,12 +122,18 @@
   <si>
     <t>Sheriff's</t>
   </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>8.15.21</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -143,6 +149,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -152,7 +165,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -225,17 +238,32 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -552,8 +580,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA2F14DC-9EA0-9F4C-829E-B310BBF5282B}">
   <dimension ref="A1:H401"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="117" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView tabSelected="1" topLeftCell="A277" zoomScale="117" workbookViewId="0">
+      <selection activeCell="D289" sqref="D289"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1791,8 +1819,12 @@
         <f t="shared" si="0"/>
         <v>53</v>
       </c>
-      <c r="B54" s="4"/>
-      <c r="C54" s="4"/>
+      <c r="B54" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="C54" s="7" t="s">
+        <v>33</v>
+      </c>
       <c r="D54" s="4" t="s">
         <v>13</v>
       </c>
@@ -2343,8 +2375,12 @@
         <f t="shared" si="1"/>
         <v>77</v>
       </c>
-      <c r="B78" s="4"/>
-      <c r="C78" s="4"/>
+      <c r="B78" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C78" s="4" t="s">
+        <v>33</v>
+      </c>
       <c r="D78" s="4" t="s">
         <v>13</v>
       </c>
@@ -2435,8 +2471,12 @@
         <f t="shared" si="1"/>
         <v>81</v>
       </c>
-      <c r="B82" s="4"/>
-      <c r="C82" s="4"/>
+      <c r="B82" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="C82" s="7" t="s">
+        <v>33</v>
+      </c>
       <c r="D82" s="4" t="s">
         <v>13</v>
       </c>
@@ -2458,8 +2498,12 @@
         <f t="shared" si="1"/>
         <v>82</v>
       </c>
-      <c r="B83" s="4"/>
-      <c r="C83" s="4"/>
+      <c r="B83" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="C83" s="7" t="s">
+        <v>33</v>
+      </c>
       <c r="D83" s="4" t="s">
         <v>12</v>
       </c>
@@ -2711,8 +2755,12 @@
         <f t="shared" si="1"/>
         <v>93</v>
       </c>
-      <c r="B94" s="4"/>
-      <c r="C94" s="4"/>
+      <c r="B94" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C94" s="4" t="s">
+        <v>33</v>
+      </c>
       <c r="D94" s="4" t="s">
         <v>13</v>
       </c>
@@ -2826,8 +2874,12 @@
         <f t="shared" si="1"/>
         <v>98</v>
       </c>
-      <c r="B99" s="4"/>
-      <c r="C99" s="4"/>
+      <c r="B99" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C99" s="4" t="s">
+        <v>33</v>
+      </c>
       <c r="D99" s="4" t="s">
         <v>12</v>
       </c>
@@ -2849,8 +2901,12 @@
         <f t="shared" si="1"/>
         <v>99</v>
       </c>
-      <c r="B100" s="4"/>
-      <c r="C100" s="4"/>
+      <c r="B100" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C100" s="4" t="s">
+        <v>33</v>
+      </c>
       <c r="D100" s="4" t="s">
         <v>12</v>
       </c>
@@ -6805,8 +6861,12 @@
         <f t="shared" si="4"/>
         <v>271</v>
       </c>
-      <c r="B272" s="4"/>
-      <c r="C272" s="4"/>
+      <c r="B272" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C272" s="4" t="s">
+        <v>33</v>
+      </c>
       <c r="D272" s="4" t="s">
         <v>12</v>
       </c>
@@ -7219,8 +7279,12 @@
         <f t="shared" si="4"/>
         <v>289</v>
       </c>
-      <c r="B290" s="4"/>
-      <c r="C290" s="4"/>
+      <c r="B290" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C290" s="4" t="s">
+        <v>33</v>
+      </c>
       <c r="D290" s="4" t="s">
         <v>12</v>
       </c>
@@ -7265,8 +7329,12 @@
         <f t="shared" si="4"/>
         <v>291</v>
       </c>
-      <c r="B292" s="4"/>
-      <c r="C292" s="4"/>
+      <c r="B292" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="C292" s="7" t="s">
+        <v>33</v>
+      </c>
       <c r="D292" s="4" t="s">
         <v>13</v>
       </c>

</xml_diff>